<commit_message>
nlp and reg models...
</commit_message>
<xml_diff>
--- a/Final_Project/data_details.xlsx
+++ b/Final_Project/data_details.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="7600" windowWidth="28800" windowHeight="8440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="116">
   <si>
     <t>Columns</t>
   </si>
@@ -359,6 +359,18 @@
   </si>
   <si>
     <t xml:space="preserve">Int </t>
+  </si>
+  <si>
+    <t>floats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">terrible </t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -458,11 +470,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="56">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -524,7 +544,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="56">
+  <cellStyles count="64">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -552,6 +572,10 @@
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -579,6 +603,10 @@
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -909,11 +937,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1005,30 +1033,6 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>38</v>
@@ -1318,7 +1322,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:12">
       <c r="A33" s="4" t="s">
         <v>69</v>
       </c>
@@ -1333,7 +1337,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:12">
       <c r="A34" s="4" t="s">
         <v>71</v>
       </c>
@@ -1348,7 +1352,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:12">
       <c r="A35" s="4" t="s">
         <v>73</v>
       </c>
@@ -1363,7 +1367,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:12">
       <c r="A36" s="5" t="s">
         <v>75</v>
       </c>
@@ -1376,7 +1380,7 @@
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:12">
       <c r="A37" s="4" t="s">
         <v>100</v>
       </c>
@@ -1393,7 +1397,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:12">
       <c r="A38" s="4" t="s">
         <v>101</v>
       </c>
@@ -1410,7 +1414,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:12">
       <c r="A39" s="4" t="s">
         <v>102</v>
       </c>
@@ -1427,7 +1431,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:12">
       <c r="A40" s="5" t="s">
         <v>52</v>
       </c>
@@ -1444,7 +1448,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:12">
       <c r="A41" s="5" t="s">
         <v>53</v>
       </c>
@@ -1461,7 +1465,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="1" customFormat="1">
+    <row r="44" spans="1:12" s="1" customFormat="1">
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
@@ -1474,8 +1478,29 @@
       <c r="D44" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1">
+        <v>2</v>
+      </c>
+      <c r="I44" s="1">
+        <v>3</v>
+      </c>
+      <c r="J44" s="1">
+        <v>4</v>
+      </c>
+      <c r="K44" s="1">
+        <v>5</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -1485,8 +1510,30 @@
       <c r="C45" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>12</v>
+      </c>
+      <c r="I45">
+        <v>39</v>
+      </c>
+      <c r="J45">
+        <v>23</v>
+      </c>
+      <c r="K45">
+        <v>2</v>
+      </c>
+      <c r="L45">
+        <f>SUM(F45:K45)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="3" t="s">
         <v>56</v>
       </c>
@@ -1498,21 +1545,65 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" t="s">
+      <c r="F46" s="3">
+        <v>4</v>
+      </c>
+      <c r="G46" s="3">
+        <v>4</v>
+      </c>
+      <c r="H46">
+        <v>18</v>
+      </c>
+      <c r="I46" s="3">
+        <v>44</v>
+      </c>
+      <c r="J46" s="3">
+        <v>68</v>
+      </c>
+      <c r="K46" s="3">
+        <v>6</v>
+      </c>
+      <c r="L46">
+        <f t="shared" ref="L46:L60" si="0">SUM(F46:K46)</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B47" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5">
+        <v>86</v>
+      </c>
+      <c r="G47" s="5">
+        <v>15</v>
+      </c>
+      <c r="H47" s="5">
+        <v>382</v>
+      </c>
+      <c r="I47" s="5">
+        <v>577</v>
+      </c>
+      <c r="J47" s="5">
+        <v>416</v>
+      </c>
+      <c r="K47" s="5">
+        <v>161</v>
+      </c>
+      <c r="L47" s="5">
+        <f t="shared" si="0"/>
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -1522,8 +1613,30 @@
       <c r="C48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="F48">
+        <v>62</v>
+      </c>
+      <c r="G48">
+        <v>7</v>
+      </c>
+      <c r="H48">
+        <v>159</v>
+      </c>
+      <c r="I48">
+        <v>308</v>
+      </c>
+      <c r="J48">
+        <v>174</v>
+      </c>
+      <c r="K48">
+        <v>78</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="0"/>
+        <v>788</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -1533,8 +1646,30 @@
       <c r="C49" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>33</v>
+      </c>
+      <c r="I49">
+        <v>78</v>
+      </c>
+      <c r="J49">
+        <v>71</v>
+      </c>
+      <c r="K49">
+        <v>30</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="0"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -1544,8 +1679,30 @@
       <c r="C50" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>7</v>
+      </c>
+      <c r="I50">
+        <v>26</v>
+      </c>
+      <c r="J50">
+        <v>25</v>
+      </c>
+      <c r="K50">
+        <v>4</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -1555,8 +1712,30 @@
       <c r="C51" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="F51">
+        <v>5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>115</v>
+      </c>
+      <c r="H51">
+        <v>14</v>
+      </c>
+      <c r="I51">
+        <v>56</v>
+      </c>
+      <c r="J51">
+        <v>39</v>
+      </c>
+      <c r="K51">
+        <v>14</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -1566,8 +1745,30 @@
       <c r="C52" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>20</v>
+      </c>
+      <c r="H52">
+        <v>65</v>
+      </c>
+      <c r="I52">
+        <v>253</v>
+      </c>
+      <c r="J52">
+        <v>143</v>
+      </c>
+      <c r="K52">
+        <v>35</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="0"/>
+        <v>517</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -1577,8 +1778,30 @@
       <c r="C53" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53">
+        <v>25</v>
+      </c>
+      <c r="I53">
+        <v>70</v>
+      </c>
+      <c r="J53">
+        <v>78</v>
+      </c>
+      <c r="K53">
+        <v>9</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="0"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -1588,19 +1811,65 @@
       <c r="C54" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>11</v>
+      </c>
+      <c r="I54">
+        <v>21</v>
+      </c>
+      <c r="J54">
+        <v>19</v>
+      </c>
+      <c r="K54">
+        <v>5</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B55" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B55" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5">
+        <v>25</v>
+      </c>
+      <c r="G55" s="5">
+        <v>35</v>
+      </c>
+      <c r="H55" s="5">
+        <v>104</v>
+      </c>
+      <c r="I55" s="5">
+        <v>445</v>
+      </c>
+      <c r="J55" s="5">
+        <v>727</v>
+      </c>
+      <c r="K55" s="5">
+        <v>54</v>
+      </c>
+      <c r="L55" s="5">
+        <f t="shared" si="0"/>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>72</v>
       </c>
@@ -1610,8 +1879,30 @@
       <c r="C56" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="F56">
+        <v>6</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>58</v>
+      </c>
+      <c r="I56">
+        <v>60</v>
+      </c>
+      <c r="J56">
+        <v>42</v>
+      </c>
+      <c r="K56">
+        <v>8</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>74</v>
       </c>
@@ -1621,8 +1912,30 @@
       <c r="C57" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="F57">
+        <v>5</v>
+      </c>
+      <c r="G57">
+        <v>6</v>
+      </c>
+      <c r="H57">
+        <v>38</v>
+      </c>
+      <c r="I57">
+        <v>165</v>
+      </c>
+      <c r="J57">
+        <v>100</v>
+      </c>
+      <c r="K57">
+        <v>27</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="0"/>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -1632,89 +1945,340 @@
       <c r="C58" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
+      <c r="F58">
+        <v>9</v>
+      </c>
+      <c r="G58">
+        <v>37</v>
+      </c>
+      <c r="H58">
+        <v>70</v>
+      </c>
+      <c r="I58">
+        <v>268</v>
+      </c>
+      <c r="J58">
+        <v>163</v>
+      </c>
+      <c r="K58">
+        <v>19</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="0"/>
+        <v>566</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B60" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
+      <c r="F60">
+        <v>526</v>
+      </c>
+      <c r="G60">
+        <v>962</v>
+      </c>
+      <c r="H60">
+        <v>1312</v>
+      </c>
+      <c r="I60">
+        <v>3870</v>
+      </c>
+      <c r="J60">
+        <v>3396</v>
+      </c>
+      <c r="K60">
+        <v>463</v>
+      </c>
+      <c r="L60">
+        <f>SUM(F60:K60)</f>
+        <v>10529</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B61" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+      <c r="F61">
+        <v>526</v>
+      </c>
+      <c r="G61">
+        <v>962</v>
+      </c>
+      <c r="H61">
+        <v>1312</v>
+      </c>
+      <c r="I61">
+        <v>3869</v>
+      </c>
+      <c r="J61">
+        <v>3396</v>
+      </c>
+      <c r="K61">
+        <v>463</v>
+      </c>
+      <c r="L61">
+        <f t="shared" ref="L61:L67" si="1">SUM(F61:K61)</f>
+        <v>10528</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B62" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+      <c r="F62">
+        <v>526</v>
+      </c>
+      <c r="G62">
+        <v>962</v>
+      </c>
+      <c r="H62">
+        <v>1312</v>
+      </c>
+      <c r="I62">
+        <v>3868</v>
+      </c>
+      <c r="J62">
+        <v>3396</v>
+      </c>
+      <c r="K62">
+        <v>463</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="1"/>
+        <v>10527</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+      <c r="F63">
+        <v>526</v>
+      </c>
+      <c r="G63">
+        <v>962</v>
+      </c>
+      <c r="H63">
+        <v>1312</v>
+      </c>
+      <c r="I63">
+        <v>3868</v>
+      </c>
+      <c r="J63">
+        <v>3396</v>
+      </c>
+      <c r="K63">
+        <v>463</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="1"/>
+        <v>10527</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B64" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" t="s">
+      <c r="F64">
+        <v>526</v>
+      </c>
+      <c r="G64">
+        <v>962</v>
+      </c>
+      <c r="H64">
+        <v>1312</v>
+      </c>
+      <c r="I64">
+        <v>3868</v>
+      </c>
+      <c r="J64">
+        <v>3396</v>
+      </c>
+      <c r="K64">
+        <v>463</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="1"/>
+        <v>10527</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B65" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" t="s">
+      <c r="F65">
+        <v>526</v>
+      </c>
+      <c r="G65">
+        <v>962</v>
+      </c>
+      <c r="H65">
+        <v>1312</v>
+      </c>
+      <c r="I65">
+        <v>3868</v>
+      </c>
+      <c r="J65">
+        <v>3396</v>
+      </c>
+      <c r="K65">
+        <v>463</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="1"/>
+        <v>10527</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="5"/>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B67" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" t="s">
+      <c r="F67">
+        <v>526</v>
+      </c>
+      <c r="G67">
+        <v>962</v>
+      </c>
+      <c r="H67">
+        <v>1312</v>
+      </c>
+      <c r="I67">
+        <v>3870</v>
+      </c>
+      <c r="J67">
+        <v>3396</v>
+      </c>
+      <c r="K67">
+        <v>463</v>
+      </c>
+      <c r="L67">
+        <f>SUM(F67:K67)</f>
+        <v>10529</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B68" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" t="s">
+      <c r="F68">
+        <v>526</v>
+      </c>
+      <c r="G68">
+        <v>960</v>
+      </c>
+      <c r="H68">
+        <v>1312</v>
+      </c>
+      <c r="I68">
+        <v>3865</v>
+      </c>
+      <c r="J68">
+        <v>3394</v>
+      </c>
+      <c r="K68">
+        <v>463</v>
+      </c>
+      <c r="L68">
+        <f t="shared" ref="L68:L70" si="2">SUM(F68:K68)</f>
+        <v>10520</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B69" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" t="s">
+      <c r="F69">
+        <v>526</v>
+      </c>
+      <c r="G69">
+        <v>960</v>
+      </c>
+      <c r="H69">
+        <v>1312</v>
+      </c>
+      <c r="I69">
+        <v>3864</v>
+      </c>
+      <c r="J69">
+        <v>3392</v>
+      </c>
+      <c r="K69">
+        <v>462</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="2"/>
+        <v>10516</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B70" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" t="s">
+      <c r="F70">
+        <v>526</v>
+      </c>
+      <c r="G70">
+        <v>960</v>
+      </c>
+      <c r="H70">
+        <v>1312</v>
+      </c>
+      <c r="I70">
+        <v>3862</v>
+      </c>
+      <c r="J70">
+        <v>3392</v>
+      </c>
+      <c r="K70">
+        <v>462</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="2"/>
+        <v>10514</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="5"/>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="5"/>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B73" t="s">
@@ -1723,16 +2287,41 @@
       <c r="C73" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" t="s">
+      <c r="F73">
+        <v>526</v>
+      </c>
+      <c r="G73">
+        <v>959</v>
+      </c>
+      <c r="H73">
+        <v>1312</v>
+      </c>
+      <c r="I73">
+        <v>3863</v>
+      </c>
+      <c r="J73">
+        <v>3392</v>
+      </c>
+      <c r="K73">
+        <v>463</v>
+      </c>
+      <c r="L73">
+        <f>SUM(F73:K73)</f>
+        <v>10515</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="5"/>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B75" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:12">
       <c r="A76" s="4" t="s">
         <v>33</v>
       </c>
@@ -1745,7 +2334,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
         <v>40</v>
       </c>
@@ -1753,7 +2342,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
         <v>41</v>
       </c>
@@ -1761,7 +2350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -1818,10 +2407,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1831,7 +2420,7 @@
     <col min="4" max="4" width="43.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1845,7 +2434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1856,7 +2445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1867,7 +2456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1875,7 +2464,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1885,6 +2474,36 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected final paper, improved datadictionary, added example html case file
</commit_message>
<xml_diff>
--- a/Final_Project/data_details.xlsx
+++ b/Final_Project/data_details.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7600" windowWidth="28800" windowHeight="8440" tabRatio="500"/>
+    <workbookView xWindow="-100" yWindow="0" windowWidth="28800" windowHeight="12360" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Features" sheetId="1" r:id="rId1"/>
-    <sheet name="Ignored Features" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Dictionary" sheetId="3" r:id="rId1"/>
+    <sheet name="Features" sheetId="1" r:id="rId2"/>
+    <sheet name="Ignored Features" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Features!$A$1:$D$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Features!$A$1:$D$84</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="173">
   <si>
     <t>Columns</t>
   </si>
@@ -371,13 +372,184 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>converted to</t>
+  </si>
+  <si>
+    <t>eg '38 years'</t>
+  </si>
+  <si>
+    <t>`'max-age'-'min_age'</t>
+  </si>
+  <si>
+    <t>l_eye</t>
+  </si>
+  <si>
+    <t>r_eye</t>
+  </si>
+  <si>
+    <t>_face</t>
+  </si>
+  <si>
+    <t>more notes</t>
+  </si>
+  <si>
+    <t>dna</t>
+  </si>
+  <si>
+    <t>fingerprints</t>
+  </si>
+  <si>
+    <t>dental</t>
+  </si>
+  <si>
+    <t>list of colors to choose</t>
+  </si>
+  <si>
+    <t>float '_min_age'</t>
+  </si>
+  <si>
+    <t>float '_max_age'</t>
+  </si>
+  <si>
+    <t>_min_age</t>
+  </si>
+  <si>
+    <t>_max_age</t>
+  </si>
+  <si>
+    <t>_sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eg, Male, Femle, Unsure, ' ' </t>
+  </si>
+  <si>
+    <t>`'n-limbs' = one or more limbs not recovered</t>
+  </si>
+  <si>
+    <t>Some options were 'pink' or 'maroon'. I counted these as '0' since they are unnatural colors</t>
+  </si>
+  <si>
+    <t>Male, Female = 1, Unsure, ' ' = 0</t>
+  </si>
+  <si>
+    <t>Recognizable' = 1, all other 'unrecognizable' or ' '  = 0</t>
+  </si>
+  <si>
+    <t>Available', 'Available elsewhere' = 1, 'Currently not available', 'No fingerprints available' = 0</t>
+  </si>
+  <si>
+    <t>similar to _dentall</t>
+  </si>
+  <si>
+    <t>similar to dental</t>
+  </si>
+  <si>
+    <t>same as l_eye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">binary: _dental  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">binary: _fingerprints  </t>
+  </si>
+  <si>
+    <t>binary: _dna</t>
+  </si>
+  <si>
+    <t>binary: l_eye</t>
+  </si>
+  <si>
+    <t>binary: r_eye</t>
+  </si>
+  <si>
+    <t>binary: _face</t>
+  </si>
+  <si>
+    <t>binary: _sex</t>
+  </si>
+  <si>
+    <t>List of text 'dropdown' options</t>
+  </si>
+  <si>
+    <t>under 30 years', 'under 50 years' etc</t>
+  </si>
+  <si>
+    <t>eg '2004 to 2009'</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Target Response</t>
+  </si>
+  <si>
+    <t>int: 0, 1, 2, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>High', 'Medium High', 'Medium', 'Low Medium', 'Low', 'Extremely Low'</t>
+  </si>
+  <si>
+    <t>e.g. '99 years'</t>
+  </si>
+  <si>
+    <t>e.g. '0\n\t\t\t\t\tWeeks'</t>
+  </si>
+  <si>
+    <t>e.g '64,\n\t\t\t\t\tEstimated' (Other text: 'Cannot Estimate', 'Measured')</t>
+  </si>
+  <si>
+    <t>eg. '198,\n\t\t\t\t\tEstimated' (Other text: 'Cannot Estimate', 'Measured'</t>
+  </si>
+  <si>
+    <t>''weight_int', 'weight_text', 'weight_bin'</t>
+  </si>
+  <si>
+    <t>`'height_int', 'height_text', 'height_bin'</t>
+  </si>
+  <si>
+    <t>weight_int</t>
+  </si>
+  <si>
+    <t>height_int</t>
+  </si>
+  <si>
+    <t>weight_bin</t>
+  </si>
+  <si>
+    <t>height_bin</t>
+  </si>
+  <si>
+    <t>Measured' or 'Estimated' = 1, 'Cannot Estimate' or ' ' = 0</t>
+  </si>
+  <si>
+    <t>made from 'weight'</t>
+  </si>
+  <si>
+    <t>made from 'height'</t>
+  </si>
+  <si>
+    <t>made from 'min_age'</t>
+  </si>
+  <si>
+    <t>made from 'max_age'</t>
+  </si>
+  <si>
+    <t>e.g. Available', 'Available elsewhere', 'Currently not available', 'No fingerprints available'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e.g. 'Recognizable' , several  'Unrecognizable' options, and  ' ' </t>
+  </si>
+  <si>
+    <t>long form text descriptions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -437,6 +609,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -470,7 +649,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -535,16 +714,66 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="112">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -576,6 +805,30 @@
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -607,6 +860,30 @@
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -937,11 +1214,1108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="60" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="18">
+      <c r="A1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="6" customFormat="1" ht="18">
+      <c r="A4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18">
+      <c r="A13" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="6" customFormat="1" ht="18">
+      <c r="A33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="18">
+      <c r="A43" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="6" customFormat="1" ht="18">
+      <c r="A44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" t="s">
+        <v>170</v>
+      </c>
+      <c r="D45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" t="s">
+        <v>171</v>
+      </c>
+      <c r="D49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" t="s">
+        <v>132</v>
+      </c>
+      <c r="D51" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="18">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="1:4" ht="18">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="58" spans="1:4" s="6" customFormat="1" ht="18">
+      <c r="A58" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" t="s">
+        <v>24</v>
+      </c>
+      <c r="C71" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" t="s">
+        <v>24</v>
+      </c>
+      <c r="C76" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" t="s">
+        <v>24</v>
+      </c>
+      <c r="C77" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" t="s">
+        <v>24</v>
+      </c>
+      <c r="C78" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" t="s">
+        <v>24</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>50</v>
+      </c>
+      <c r="B82" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>51</v>
+      </c>
+      <c r="B83" t="s">
+        <v>24</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>54</v>
+      </c>
+      <c r="B85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>46</v>
+      </c>
+      <c r="B87" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" s="1" customFormat="1" ht="18">
+      <c r="A89" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>40</v>
+      </c>
+      <c r="B90" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>41</v>
+      </c>
+      <c r="B91" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>42</v>
+      </c>
+      <c r="B92" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>43</v>
+      </c>
+      <c r="B93" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>44</v>
+      </c>
+      <c r="B94" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>45</v>
+      </c>
+      <c r="B95" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>23</v>
+      </c>
+      <c r="B97" t="s">
+        <v>24</v>
+      </c>
+      <c r="C97" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>29</v>
+      </c>
+      <c r="B98" t="s">
+        <v>24</v>
+      </c>
+      <c r="C98" t="s">
+        <v>117</v>
+      </c>
+      <c r="D98" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>30</v>
+      </c>
+      <c r="B99" t="s">
+        <v>24</v>
+      </c>
+      <c r="C99" t="s">
+        <v>155</v>
+      </c>
+      <c r="D99" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>38</v>
+      </c>
+      <c r="B101" t="s">
+        <v>24</v>
+      </c>
+      <c r="C101" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>34</v>
+      </c>
+      <c r="B102" t="s">
+        <v>24</v>
+      </c>
+      <c r="C102" t="s">
+        <v>158</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>35</v>
+      </c>
+      <c r="B103" t="s">
+        <v>24</v>
+      </c>
+      <c r="C103" t="s">
+        <v>157</v>
+      </c>
+      <c r="D103" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>39</v>
+      </c>
+      <c r="B104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C104" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J55" sqref="J55"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B87" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -980,17 +2354,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
-    </row>
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>29</v>
@@ -1033,30 +2396,6 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
     <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>13</v>
@@ -1564,7 +2903,7 @@
         <v>6</v>
       </c>
       <c r="L46">
-        <f t="shared" ref="L46:L60" si="0">SUM(F46:K46)</f>
+        <f t="shared" ref="L46:L58" si="0">SUM(F46:K46)</f>
         <v>144</v>
       </c>
     </row>
@@ -2024,7 +3363,7 @@
         <v>463</v>
       </c>
       <c r="L61">
-        <f t="shared" ref="L61:L67" si="1">SUM(F61:K61)</f>
+        <f t="shared" ref="L61:L65" si="1">SUM(F61:K61)</f>
         <v>10528</v>
       </c>
     </row>
@@ -2332,54 +3671,6 @@
       <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12">
-      <c r="A78" t="s">
-        <v>40</v>
-      </c>
-      <c r="B78" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12">
-      <c r="A79" t="s">
-        <v>41</v>
-      </c>
-      <c r="B79" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12">
-      <c r="A80" t="s">
-        <v>42</v>
-      </c>
-      <c r="B80" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>43</v>
-      </c>
-      <c r="B81" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>44</v>
-      </c>
-      <c r="B82" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>45</v>
-      </c>
-      <c r="B83" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2405,12 +3696,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A2" sqref="A2:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2506,8 +3797,92 @@
         <v>113</v>
       </c>
     </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>